<commit_message>
good: save in excel file
</commit_message>
<xml_diff>
--- a/UNIDADE.xlsx
+++ b/UNIDADE.xlsx
@@ -443,12 +443,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Nome Unidade</t>
+          <t>Nome</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Salas</t>
+          <t>chave</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">

</xml_diff>